<commit_message>
+ add a tri-state buffer to connect `MEM_SO` to `USB_SI` only when the FTDI is programming the Flash
</commit_message>
<xml_diff>
--- a/hardware/development/clear-dev-v1/clear-dev-v1.xlsx
+++ b/hardware/development/clear-dev-v1/clear-dev-v1.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">SN74LVC1G125DCKT</t>
   </si>
   <si>
-    <t xml:space="preserve">U2, U3</t>
+    <t xml:space="preserve">U2, U3, U4</t>
   </si>
   <si>
     <t xml:space="preserve">Mouser</t>
@@ -547,7 +547,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -619,7 +619,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
update clear dev BOM
</commit_message>
<xml_diff>
--- a/hardware/development/clear-dev-v1/clear-dev-v1.xlsx
+++ b/hardware/development/clear-dev-v1/clear-dev-v1.xlsx
@@ -88,13 +88,13 @@
     <t xml:space="preserve">U6</t>
   </si>
   <si>
+    <t xml:space="preserve">1.8v</t>
+  </si>
+  <si>
     <t xml:space="preserve">W25Q32JVSSIQ</t>
   </si>
   <si>
     <t xml:space="preserve">U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.8v</t>
   </si>
   <si>
     <t xml:space="preserve">M.2 E connector</t>
@@ -547,7 +547,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -674,19 +674,22 @@
       <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>11</v>
@@ -694,9 +697,7 @@
       <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="I6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="n">

</xml_diff>